<commit_message>
mehr von Unit 6
</commit_message>
<xml_diff>
--- a/englisch_6_unit5_6.xlsx
+++ b/englisch_6_unit5_6.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
   <si>
     <t xml:space="preserve">youth hostel</t>
   </si>
@@ -281,6 +281,276 @@
   </si>
   <si>
     <t xml:space="preserve">Briefkasten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weather </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wetter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to promise</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> versprechen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">call</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anruf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hiker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wanderer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wanderung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to jope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hoffen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">office</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Büro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wenn,falls,ob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">helicopter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helikopter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nachricht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thunderstorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gewitter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">worker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arbeiter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arbeit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nebel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foggy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">neblig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to land</t>
+  </si>
+  <si>
+    <t xml:space="preserve">landen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">warning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warnung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Woolke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cloudy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wolkig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sunny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sonnig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spinne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Held</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Höhle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">battle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schlacht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soldier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soldat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prisoner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gefangener</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to kill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">töten, umbringen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gentle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sanft,liebenswürdig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hot-headed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hitzköpfig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geduldig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fight,fought,fought</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kämpfen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(not) any longer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(nicht) mehr, (nicht) länger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ride, rode,ridden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reiten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Netz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">again and again</t>
+  </si>
+  <si>
+    <t xml:space="preserve">immer wieder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dünn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schwach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nett, freundlich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to share</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teilen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wife</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ehefrau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">daughter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tochter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perfect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perfekt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charakter</t>
   </si>
 </sst>
 </file>
@@ -289,13 +559,14 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;WAHR&quot;;&quot;WAHR&quot;;&quot;FALSCH&quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot;LO&quot;G\IS\CH"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -311,6 +582,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -355,7 +631,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -366,6 +642,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -385,15 +665,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B89" activeCellId="0" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.87"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
@@ -610,7 +890,8 @@
       <c r="A27" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="1" t="b">
+      <c r="B27" s="1" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -748,6 +1029,366 @@
       </c>
       <c r="B44" s="0" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>